<commit_message>
+Completed the question with exception handling and annotations
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Day11_Assignment2\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\UiPath\Shireen_Day11_Assignment2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241F4ADB-D623-4704-A3D7-AFBB7A62622E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1F32B2-D374-4589-97E0-EFA76312A0E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -167,6 +167,42 @@
   </si>
   <si>
     <t>Data\Input\Question1.xlsx</t>
+  </si>
+  <si>
+    <t>TimeOut</t>
+  </si>
+  <si>
+    <t>Url of the botsdna browser</t>
+  </si>
+  <si>
+    <t>Delay time for the check app state activity</t>
+  </si>
+  <si>
+    <t>SystemException</t>
+  </si>
+  <si>
+    <t>Browser not loading</t>
+  </si>
+  <si>
+    <t>BusinessException</t>
+  </si>
+  <si>
+    <t>Server not found</t>
+  </si>
+  <si>
+    <t>Exception message to display in case of system exception</t>
+  </si>
+  <si>
+    <t>Exception message to display in case of Business exception</t>
+  </si>
+  <si>
+    <t>OutputSheet</t>
+  </si>
+  <si>
+    <t>Name of the sheet where the output excel will be written</t>
+  </si>
+  <si>
+    <t>Sheet3</t>
   </si>
 </sst>
 </file>
@@ -246,9 +282,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -286,7 +322,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -392,7 +428,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -534,7 +570,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -548,12 +584,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -601,7 +637,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" ht="14.5">
       <c r="A3" s="2" t="s">
         <v>42</v>
       </c>
@@ -613,7 +649,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1629,15 +1665,15 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1674,7 +1710,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1685,7 +1721,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1799,7 +1835,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1817,11 +1853,54 @@
       <c r="B18" t="s">
         <v>39</v>
       </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2800,12 +2879,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>